<commit_message>
Added working time of this day
</commit_message>
<xml_diff>
--- a/Dokumentation/arbeitszeiten/Arbeitszeiten_grr37213.xlsx
+++ b/Dokumentation/arbeitszeiten/Arbeitszeiten_grr37213.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t xml:space="preserve">Arbeitszeit je Woche:</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Projektbeschreibung / Terminplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Sollstunden:</t>
@@ -225,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,10 +265,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,10 +317,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,22 +325,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,16 +333,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -400,18 +375,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -435,357 +398,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -920,7 +533,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF9C6500"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFD9D9D9"/>
@@ -944,7 +557,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFC6EFCE"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFEB9C"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -983,10 +596,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +645,7 @@
       </c>
       <c r="B7" s="8" t="n">
         <f aca="false">'Oktober 2017'!G34</f>
-        <v>1.6</v>
+        <v>9.16666666666667</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">'Oktober 2017'!C33</f>
@@ -1073,7 +686,7 @@
         <f aca="false">'Januar 2018'!G34</f>
         <v>0</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">'Januar 2018'!C33</f>
         <v>45</v>
       </c>
@@ -1081,15 +694,14 @@
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="8" t="n">
         <f aca="false">SUM(B7:B9)</f>
-        <v>1.6</v>
+        <v>9.16666666666667</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">SUM(C7:C10)</f>
@@ -1115,181 +727,182 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.61395348837209"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
+      <c r="A2" s="11" t="n">
         <f aca="false">DATE(2017,10,1)</f>
         <v>43009</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="12" t="n">
         <f aca="false">A2</f>
         <v>43009</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="13" t="n">
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>40</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16" t="n">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15" t="n">
         <f aca="false">(E2-D2-F2)*24</f>
         <v>0</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
+      <c r="A3" s="11" t="n">
         <f aca="false">A2+1</f>
         <v>43010</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="12" t="n">
         <f aca="false">A3</f>
         <v>43010</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="13" t="n">
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>41</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16" t="n">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15" t="n">
         <f aca="false">(E3-D3-F3)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+      <c r="A4" s="11" t="n">
         <f aca="false">A3+1</f>
         <v>43011</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="12" t="n">
         <f aca="false">A4</f>
         <v>43011</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="13" t="n">
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>41</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16" t="n">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15" t="n">
         <f aca="false">(E4-D4-F4)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="11" t="n">
         <f aca="false">A4+1</f>
         <v>43012</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="12" t="n">
         <f aca="false">A5</f>
         <v>43012</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C5" s="13" t="n">
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>41</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16" t="n">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15" t="n">
         <f aca="false">(E5-D5-F5)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="11" t="n">
         <f aca="false">A5+1</f>
         <v>43013</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="n">
+      <c r="C6" s="13" t="n">
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>41</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16" t="n">
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15" t="n">
         <f aca="false">(E6-D6-F6)*24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="23" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="n">
+    <row r="7" s="19" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="n">
         <f aca="false">A6+1</f>
         <v>43014</v>
       </c>
-      <c r="B7" s="19" t="n">
+      <c r="B7" s="18" t="n">
         <f aca="false">A7</f>
         <v>43014</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="19" t="n">
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>41</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="20" t="n">
         <v>0.510416666666667</v>
       </c>
-      <c r="E7" s="21" t="n">
+      <c r="E7" s="20" t="n">
         <v>0.572916666666667</v>
       </c>
-      <c r="F7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22" t="n">
+      <c r="F7" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="21" t="n">
         <f aca="false">(E7-D7-F7)*24</f>
         <v>1.5</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1298,17 +911,17 @@
         <f aca="false">A7+1</f>
         <v>43015</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <f aca="false">A8</f>
         <v>43015</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>41</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="8" t="n">
         <f aca="false">(E8-D8-F8)*24</f>
         <v>0</v>
@@ -1320,17 +933,17 @@
         <f aca="false">A8+1</f>
         <v>43016</v>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="22" t="n">
         <f aca="false">A9</f>
         <v>43016</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>41</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="8" t="n">
         <f aca="false">(E9-D9-F9)*24</f>
         <v>0</v>
@@ -1342,17 +955,17 @@
         <f aca="false">A9+1</f>
         <v>43017</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="22" t="n">
         <f aca="false">A10</f>
         <v>43017</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>42</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="8" t="n">
         <f aca="false">(E10-D10-F10)*24</f>
         <v>0</v>
@@ -1363,18 +976,18 @@
         <f aca="false">A10+1</f>
         <v>43018</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="22" t="n">
         <f aca="false">A11</f>
         <v>43018</v>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="0" t="n">
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>42</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="8" t="n">
         <f aca="false">(E11-D11-F11)*24</f>
         <v>0</v>
       </c>
@@ -1384,18 +997,18 @@
         <f aca="false">A11+1</f>
         <v>43019</v>
       </c>
-      <c r="B12" s="26" t="n">
+      <c r="B12" s="22" t="n">
         <f aca="false">A12</f>
         <v>43019</v>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="0" t="n">
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>42</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="8" t="n">
         <f aca="false">(E12-D12-F12)*24</f>
         <v>0</v>
       </c>
@@ -1405,58 +1018,58 @@
         <f aca="false">A12+1</f>
         <v>43020</v>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="22" t="n">
         <f aca="false">A13</f>
         <v>43020</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="0" t="n">
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>42</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="8" t="n">
         <f aca="false">(E13-D13-F13)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="n">
+      <c r="A14" s="24" t="n">
         <f aca="false">A13+1</f>
         <v>43021</v>
       </c>
-      <c r="B14" s="31" t="n">
+      <c r="B14" s="25" t="n">
         <f aca="false">A14</f>
         <v>43021</v>
       </c>
-      <c r="C14" s="32" t="n">
+      <c r="C14" s="1" t="n">
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>42</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <f aca="false">A14+1</f>
         <v>43022</v>
       </c>
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="22" t="n">
         <f aca="false">A15</f>
         <v>43022</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="0" t="n">
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>42</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="8" t="n">
         <f aca="false">(E15-D15-F15)*24</f>
         <v>0</v>
@@ -1468,17 +1081,17 @@
         <f aca="false">A15+1</f>
         <v>43023</v>
       </c>
-      <c r="B16" s="24" t="n">
+      <c r="B16" s="22" t="n">
         <f aca="false">A16</f>
         <v>43023</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="0" t="n">
         <f aca="false">WEEKNUM(A16,2)</f>
         <v>42</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="8" t="n">
         <f aca="false">(E16-D16-F16)*24</f>
         <v>0</v>
@@ -1490,17 +1103,17 @@
         <f aca="false">A16+1</f>
         <v>43024</v>
       </c>
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="22" t="n">
         <f aca="false">A17</f>
         <v>43024</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="0" t="n">
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>43</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="8" t="n">
         <f aca="false">(E17-D17-F17)*24</f>
         <v>0</v>
@@ -1512,18 +1125,18 @@
         <f aca="false">A17+1</f>
         <v>43025</v>
       </c>
-      <c r="B18" s="26" t="n">
+      <c r="B18" s="22" t="n">
         <f aca="false">A18</f>
         <v>43025</v>
       </c>
-      <c r="C18" s="27" t="n">
+      <c r="C18" s="0" t="n">
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>43</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29" t="n">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="8" t="n">
         <v>0.1</v>
       </c>
       <c r="I18" s="0" t="s">
@@ -1535,79 +1148,98 @@
         <f aca="false">A18+1</f>
         <v>43026</v>
       </c>
-      <c r="B19" s="26" t="n">
+      <c r="B19" s="22" t="n">
         <f aca="false">A19</f>
         <v>43026</v>
       </c>
-      <c r="C19" s="27" t="n">
+      <c r="C19" s="0" t="n">
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>43</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29" t="n">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="8" t="n">
         <f aca="false">(E19-D19-F19)*24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <f aca="false">A19+1</f>
         <v>43027</v>
       </c>
-      <c r="B20" s="24" t="n">
+      <c r="B20" s="22" t="n">
         <f aca="false">A20</f>
         <v>43027</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="0" t="n">
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>43</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="23" t="n">
+        <v>0.68125</v>
+      </c>
+      <c r="E20" s="23" t="n">
+        <v>0.979166666666667</v>
+      </c>
+      <c r="F20" s="23" t="n">
+        <v>0.125</v>
+      </c>
       <c r="G20" s="8" t="n">
         <f aca="false">(E20-D20-F20)*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="n">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24" t="n">
         <f aca="false">A20+1</f>
         <v>43028</v>
       </c>
-      <c r="B21" s="31" t="n">
+      <c r="B21" s="25" t="n">
         <f aca="false">A21</f>
         <v>43028</v>
       </c>
-      <c r="C21" s="32" t="n">
+      <c r="C21" s="1" t="n">
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>43</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="23" t="n">
+        <v>0.688888888888889</v>
+      </c>
+      <c r="E21" s="23" t="n">
+        <v>0.89375</v>
+      </c>
+      <c r="F21" s="23" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G21" s="8" t="n">
+        <f aca="false">(E21-D21-F21)*24</f>
+        <v>3.41666666666667</v>
+      </c>
+      <c r="I21" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <f aca="false">A21+1</f>
         <v>43029</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="22" t="n">
         <f aca="false">A22</f>
         <v>43029</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="0" t="n">
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>43</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="8" t="n">
         <f aca="false">(E22-D22-F22)*24</f>
         <v>0</v>
@@ -1619,17 +1251,17 @@
         <f aca="false">A22+1</f>
         <v>43030</v>
       </c>
-      <c r="B23" s="24" t="n">
+      <c r="B23" s="22" t="n">
         <f aca="false">A23</f>
         <v>43030</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="0" t="n">
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>43</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="8" t="n">
         <f aca="false">(E23-D23-F23)*24</f>
         <v>0</v>
@@ -1641,17 +1273,17 @@
         <f aca="false">A23+1</f>
         <v>43031</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="22" t="n">
         <f aca="false">A24</f>
         <v>43031</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="0" t="n">
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>44</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="8" t="n">
         <f aca="false">(E24-D24-F24)*24</f>
         <v>0</v>
@@ -1662,18 +1294,18 @@
         <f aca="false">A24+1</f>
         <v>43032</v>
       </c>
-      <c r="B25" s="26" t="n">
+      <c r="B25" s="22" t="n">
         <f aca="false">A25</f>
         <v>43032</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="0" t="n">
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>44</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29" t="n">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="8" t="n">
         <f aca="false">(E25-D25-F25)*24</f>
         <v>0</v>
       </c>
@@ -1683,18 +1315,18 @@
         <f aca="false">A25+1</f>
         <v>43033</v>
       </c>
-      <c r="B26" s="26" t="n">
+      <c r="B26" s="22" t="n">
         <f aca="false">A26</f>
         <v>43033</v>
       </c>
-      <c r="C26" s="27" t="n">
+      <c r="C26" s="0" t="n">
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>44</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29" t="n">
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="8" t="n">
         <f aca="false">(E26-D26-F26)*24</f>
         <v>0</v>
       </c>
@@ -1704,17 +1336,17 @@
         <f aca="false">A26+1</f>
         <v>43034</v>
       </c>
-      <c r="B27" s="24" t="n">
+      <c r="B27" s="22" t="n">
         <f aca="false">A27</f>
         <v>43034</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="0" t="n">
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>44</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="8" t="n">
         <f aca="false">(E27-D27-F27)*24</f>
         <v>0</v>
@@ -1725,38 +1357,37 @@
         <f aca="false">A27+1</f>
         <v>43035</v>
       </c>
-      <c r="B28" s="24" t="n">
+      <c r="B28" s="22" t="n">
         <f aca="false">A28</f>
         <v>43035</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>44</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="8" t="n">
         <f aca="false">(E28-D28-F28)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="n">
-        <f aca="false">A28+1</f>
-        <v>43036</v>
-      </c>
-      <c r="B29" s="24" t="n">
+      <c r="A29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="22" t="str">
         <f aca="false">A29</f>
-        <v>43036</v>
-      </c>
-      <c r="C29" s="9" t="n">
+        <v> </v>
+      </c>
+      <c r="C29" s="0" t="e">
         <f aca="false">WEEKNUM(A29,2)</f>
-        <v>44</v>
-      </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="8" t="n">
         <f aca="false">(E29-D29-F29)*24</f>
         <v>0</v>
@@ -1764,21 +1395,21 @@
       <c r="H29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="4" t="e">
         <f aca="false">A29+1</f>
-        <v>43037</v>
-      </c>
-      <c r="B30" s="24" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B30" s="22" t="e">
         <f aca="false">A30</f>
-        <v>43037</v>
-      </c>
-      <c r="C30" s="9" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C30" s="0" t="e">
         <f aca="false">WEEKNUM(A30,2)</f>
-        <v>44</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="8" t="n">
         <f aca="false">(E30-D30-F30)*24</f>
         <v>0</v>
@@ -1786,53 +1417,53 @@
       <c r="H30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="4" t="e">
         <f aca="false">A30+1</f>
-        <v>43038</v>
-      </c>
-      <c r="B31" s="24" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B31" s="22" t="e">
         <f aca="false">A31</f>
-        <v>43038</v>
-      </c>
-      <c r="C31" s="9" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C31" s="0" t="e">
         <f aca="false">WEEKNUM(A31,2)</f>
-        <v>45</v>
-      </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="8" t="n">
         <f aca="false">(E31-D31-F31)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35" t="n">
+      <c r="A32" s="28" t="e">
         <f aca="false">A31+1</f>
-        <v>43039</v>
-      </c>
-      <c r="B32" s="36" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B32" s="29" t="e">
         <f aca="false">A32</f>
-        <v>43039</v>
-      </c>
-      <c r="C32" s="37" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C32" s="30" t="e">
         <f aca="false">WEEKNUM(A32,2)</f>
-        <v>45</v>
-      </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32" t="n">
         <f aca="false">(E32-D32-F32)*24</f>
         <v>0</v>
       </c>
-      <c r="H32" s="39"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="40"/>
+      <c r="A33" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="33"/>
       <c r="C33" s="0" t="n">
         <f aca="false">3*Zusammenfassung!B1</f>
         <v>27</v>
@@ -1840,87 +1471,82 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43" t="n">
+      <c r="A34" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36" t="n">
         <f aca="false">SUM(G2:G32)</f>
-        <v>1.6</v>
-      </c>
-      <c r="H34" s="43"/>
+        <v>9.16666666666667</v>
+      </c>
+      <c r="H34" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="I21:L21"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C32">
     <cfRule type="timePeriod" priority="2" timePeriod="yesterday" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G13,A22:G32,A21:D21,A15:G20,A14:D14">
+  <conditionalFormatting sqref="H8">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>WEEKDAY($A8,2) &gt; 5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>WEEKDAY($A8,2) &gt; 5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H9">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>WEEKDAY($A2,2) &gt; 5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>WEEKDAY($A9,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>WEEKDAY($A15,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>WEEKDAY($A16,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>WEEKDAY($A22,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>WEEKDAY($A23,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>WEEKDAY($A29,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>WEEKDAY($A30,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1947,39 +1573,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1988,17 +1614,17 @@
         <f aca="false">DATE(2017,11,1)</f>
         <v>43040</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="22" t="n">
         <f aca="false">A2</f>
         <v>43040</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="0" t="n">
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>45</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="8" t="n">
         <f aca="false">(E2-D2-F2)*24</f>
         <v>0</v>
@@ -2009,17 +1635,17 @@
         <f aca="false">A2+1</f>
         <v>43041</v>
       </c>
-      <c r="B3" s="24" t="n">
+      <c r="B3" s="22" t="n">
         <f aca="false">A3</f>
         <v>43041</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="0" t="n">
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>45</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="8" t="n">
         <f aca="false">(E3-D3-F3)*24</f>
         <v>0</v>
@@ -2030,18 +1656,18 @@
         <f aca="false">A3+1</f>
         <v>43042</v>
       </c>
-      <c r="B4" s="26" t="n">
+      <c r="B4" s="22" t="n">
         <f aca="false">A4</f>
         <v>43042</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="0" t="n">
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>45</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="8" t="n">
         <f aca="false">(E4-D4-F4)*24</f>
         <v>0</v>
       </c>
@@ -2051,18 +1677,18 @@
         <f aca="false">A4+1</f>
         <v>43043</v>
       </c>
-      <c r="B5" s="26" t="n">
+      <c r="B5" s="22" t="n">
         <f aca="false">A5</f>
         <v>43043</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="0" t="n">
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>45</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="8" t="n">
         <f aca="false">(E5-D5-F5)*24</f>
         <v>0</v>
       </c>
@@ -2073,17 +1699,17 @@
         <f aca="false">A5+1</f>
         <v>43044</v>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="22" t="n">
         <f aca="false">A6</f>
         <v>43044</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>45</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="8" t="n">
         <f aca="false">(E6-D6-F6)*24</f>
         <v>0</v>
@@ -2095,17 +1721,17 @@
         <f aca="false">A6+1</f>
         <v>43045</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="22" t="n">
         <f aca="false">A7</f>
         <v>43045</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>46</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="8" t="n">
         <f aca="false">(E7-D7-F7)*24</f>
         <v>0</v>
@@ -2116,17 +1742,17 @@
         <f aca="false">A7+1</f>
         <v>43046</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <f aca="false">A8</f>
         <v>43046</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>46</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="8" t="n">
         <f aca="false">(E8-D8-F8)*24</f>
         <v>0</v>
@@ -2137,17 +1763,17 @@
         <f aca="false">A8+1</f>
         <v>43047</v>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="22" t="n">
         <f aca="false">A9</f>
         <v>43047</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>46</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="8" t="n">
         <f aca="false">(E9-D9-F9)*24</f>
         <v>0</v>
@@ -2158,17 +1784,17 @@
         <f aca="false">A9+1</f>
         <v>43048</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="22" t="n">
         <f aca="false">A10</f>
         <v>43048</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>46</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="8" t="n">
         <f aca="false">(E10-D10-F10)*24</f>
         <v>0</v>
@@ -2179,18 +1805,18 @@
         <f aca="false">A10+1</f>
         <v>43049</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="22" t="n">
         <f aca="false">A11</f>
         <v>43049</v>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="0" t="n">
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>46</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="8" t="n">
         <f aca="false">(E11-D11-F11)*24</f>
         <v>0</v>
       </c>
@@ -2200,18 +1826,18 @@
         <f aca="false">A11+1</f>
         <v>43050</v>
       </c>
-      <c r="B12" s="26" t="n">
+      <c r="B12" s="22" t="n">
         <f aca="false">A12</f>
         <v>43050</v>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="0" t="n">
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>46</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="8" t="n">
         <f aca="false">(E12-D12-F12)*24</f>
         <v>0</v>
       </c>
@@ -2222,17 +1848,17 @@
         <f aca="false">A12+1</f>
         <v>43051</v>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="22" t="n">
         <f aca="false">A13</f>
         <v>43051</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="0" t="n">
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>46</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="8" t="n">
         <f aca="false">(E13-D13-F13)*24</f>
         <v>0</v>
@@ -2244,17 +1870,17 @@
         <f aca="false">A13+1</f>
         <v>43052</v>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="22" t="n">
         <f aca="false">A14</f>
         <v>43052</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>47</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="8" t="n">
         <f aca="false">(E14-D14-F14)*24</f>
         <v>0</v>
@@ -2265,17 +1891,17 @@
         <f aca="false">A14+1</f>
         <v>43053</v>
       </c>
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="22" t="n">
         <f aca="false">A15</f>
         <v>43053</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="0" t="n">
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>47</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="8" t="n">
         <f aca="false">(E15-D15-F15)*24</f>
         <v>0</v>
@@ -2286,17 +1912,17 @@
         <f aca="false">A15+1</f>
         <v>43054</v>
       </c>
-      <c r="B16" s="24" t="n">
+      <c r="B16" s="22" t="n">
         <f aca="false">A16</f>
         <v>43054</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="0" t="n">
         <f aca="false">WEEKNUM(A16,2)</f>
         <v>47</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="8" t="n">
         <f aca="false">(E16-D16-F16)*24</f>
         <v>0</v>
@@ -2307,59 +1933,59 @@
         <f aca="false">A16+1</f>
         <v>43055</v>
       </c>
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="22" t="n">
         <f aca="false">A17</f>
         <v>43055</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="0" t="n">
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>47</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="8" t="n">
         <f aca="false">(E17-D17-F17)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="n">
+      <c r="A18" s="24" t="n">
         <f aca="false">A17+1</f>
         <v>43056</v>
       </c>
-      <c r="B18" s="44" t="n">
+      <c r="B18" s="25" t="n">
         <f aca="false">A18</f>
         <v>43056</v>
       </c>
-      <c r="C18" s="45" t="n">
+      <c r="C18" s="1" t="n">
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>47</v>
       </c>
-      <c r="D18" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
+      <c r="D18" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <f aca="false">A18+1</f>
         <v>43057</v>
       </c>
-      <c r="B19" s="26" t="n">
+      <c r="B19" s="22" t="n">
         <f aca="false">A19</f>
         <v>43057</v>
       </c>
-      <c r="C19" s="27" t="n">
+      <c r="C19" s="0" t="n">
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>47</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29" t="n">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="8" t="n">
         <f aca="false">(E19-D19-F19)*24</f>
         <v>0</v>
       </c>
@@ -2370,17 +1996,17 @@
         <f aca="false">A19+1</f>
         <v>43058</v>
       </c>
-      <c r="B20" s="24" t="n">
+      <c r="B20" s="22" t="n">
         <f aca="false">A20</f>
         <v>43058</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="0" t="n">
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>47</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="8" t="n">
         <f aca="false">(E20-D20-F20)*24</f>
         <v>0</v>
@@ -2392,17 +2018,17 @@
         <f aca="false">A20+1</f>
         <v>43059</v>
       </c>
-      <c r="B21" s="24" t="n">
+      <c r="B21" s="22" t="n">
         <f aca="false">A21</f>
         <v>43059</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="0" t="n">
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>48</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="8" t="n">
         <f aca="false">(E21-D21-F21)*24</f>
         <v>0</v>
@@ -2413,17 +2039,17 @@
         <f aca="false">A21+1</f>
         <v>43060</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="22" t="n">
         <f aca="false">A22</f>
         <v>43060</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="0" t="n">
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>48</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="8" t="n">
         <f aca="false">(E22-D22-F22)*24</f>
         <v>0</v>
@@ -2434,17 +2060,17 @@
         <f aca="false">A22+1</f>
         <v>43061</v>
       </c>
-      <c r="B23" s="24" t="n">
+      <c r="B23" s="22" t="n">
         <f aca="false">A23</f>
         <v>43061</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="0" t="n">
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>48</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="8" t="n">
         <f aca="false">(E23-D23-F23)*24</f>
         <v>0</v>
@@ -2455,17 +2081,17 @@
         <f aca="false">A23+1</f>
         <v>43062</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="22" t="n">
         <f aca="false">A24</f>
         <v>43062</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="0" t="n">
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>48</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="8" t="n">
         <f aca="false">(E24-D24-F24)*24</f>
         <v>0</v>
@@ -2476,18 +2102,18 @@
         <f aca="false">A24+1</f>
         <v>43063</v>
       </c>
-      <c r="B25" s="26" t="n">
+      <c r="B25" s="22" t="n">
         <f aca="false">A25</f>
         <v>43063</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="0" t="n">
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>48</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29" t="n">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="8" t="n">
         <f aca="false">(E25-D25-F25)*24</f>
         <v>0</v>
       </c>
@@ -2497,18 +2123,18 @@
         <f aca="false">A25+1</f>
         <v>43064</v>
       </c>
-      <c r="B26" s="26" t="n">
+      <c r="B26" s="22" t="n">
         <f aca="false">A26</f>
         <v>43064</v>
       </c>
-      <c r="C26" s="27" t="n">
+      <c r="C26" s="0" t="n">
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>48</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29" t="n">
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="8" t="n">
         <f aca="false">(E26-D26-F26)*24</f>
         <v>0</v>
       </c>
@@ -2519,17 +2145,17 @@
         <f aca="false">A26+1</f>
         <v>43065</v>
       </c>
-      <c r="B27" s="24" t="n">
+      <c r="B27" s="22" t="n">
         <f aca="false">A27</f>
         <v>43065</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="0" t="n">
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>48</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="8" t="n">
         <f aca="false">(E27-D27-F27)*24</f>
         <v>0</v>
@@ -2541,17 +2167,17 @@
         <f aca="false">A27+1</f>
         <v>43066</v>
       </c>
-      <c r="B28" s="24" t="n">
+      <c r="B28" s="22" t="n">
         <f aca="false">A28</f>
         <v>43066</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>49</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="8" t="n">
         <f aca="false">(E28-D28-F28)*24</f>
         <v>0</v>
@@ -2562,17 +2188,17 @@
         <f aca="false">A28+1</f>
         <v>43067</v>
       </c>
-      <c r="B29" s="24" t="n">
+      <c r="B29" s="22" t="n">
         <f aca="false">A29</f>
         <v>43067</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="0" t="n">
         <f aca="false">WEEKNUM(A29,2)</f>
         <v>49</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="8" t="n">
         <f aca="false">(E29-D29-F29)*24</f>
         <v>0</v>
@@ -2583,17 +2209,17 @@
         <f aca="false">A29+1</f>
         <v>43068</v>
       </c>
-      <c r="B30" s="24" t="n">
+      <c r="B30" s="22" t="n">
         <f aca="false">A30</f>
         <v>43068</v>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="0" t="n">
         <f aca="false">WEEKNUM(A30,2)</f>
         <v>49</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="8" t="n">
         <f aca="false">(E30-D30-F30)*24</f>
         <v>0</v>
@@ -2604,37 +2230,37 @@
         <f aca="false">A30+1</f>
         <v>43069</v>
       </c>
-      <c r="B31" s="24" t="n">
+      <c r="B31" s="22" t="n">
         <f aca="false">A31</f>
         <v>43069</v>
       </c>
-      <c r="C31" s="9" t="n">
+      <c r="C31" s="0" t="n">
         <f aca="false">WEEKNUM(A31,2)</f>
         <v>49</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="8" t="n">
         <f aca="false">(E31-D31-F31)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="47"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="40"/>
+      <c r="A33" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="33"/>
       <c r="C33" s="0" t="n">
         <f aca="false">5*Zusammenfassung!B1</f>
         <v>45</v>
@@ -2642,19 +2268,19 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43" t="n">
+      <c r="A34" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="43"/>
+      <c r="H34" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2665,53 +2291,48 @@
   <conditionalFormatting sqref="B2:C32">
     <cfRule type="timePeriod" priority="2" timePeriod="yesterday" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G17,A19:G32,A18:D18">
+  <conditionalFormatting sqref="H5">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>WEEKDAY($A2,2) &gt; 5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A5,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A6,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>WEEKDAY($A12,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>WEEKDAY($A13,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>WEEKDAY($A19,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>WEEKDAY($A20,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>WEEKDAY($A26,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>WEEKDAY($A27,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2738,59 +2359,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="48"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <f aca="false">DATE(2017,12,1)</f>
         <v>43070</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="22" t="n">
         <f aca="false">A2</f>
         <v>43070</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="0" t="n">
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>49</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="8" t="n">
         <f aca="false">(E2-D2-F2)*24</f>
         <v>0</v>
@@ -2801,17 +2422,17 @@
         <f aca="false">A2+1</f>
         <v>43071</v>
       </c>
-      <c r="B3" s="24" t="n">
+      <c r="B3" s="22" t="n">
         <f aca="false">A3</f>
         <v>43071</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="0" t="n">
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>49</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="8" t="n">
         <f aca="false">(E3-D3-F3)*24</f>
         <v>0</v>
@@ -2823,18 +2444,18 @@
         <f aca="false">A3+1</f>
         <v>43072</v>
       </c>
-      <c r="B4" s="26" t="n">
+      <c r="B4" s="22" t="n">
         <f aca="false">A4</f>
         <v>43072</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="0" t="n">
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>49</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="8" t="n">
         <f aca="false">(E4-D4-F4)*24</f>
         <v>0</v>
       </c>
@@ -2845,18 +2466,18 @@
         <f aca="false">A4+1</f>
         <v>43073</v>
       </c>
-      <c r="B5" s="26" t="n">
+      <c r="B5" s="22" t="n">
         <f aca="false">A5</f>
         <v>43073</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="0" t="n">
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>50</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="8" t="n">
         <f aca="false">(E5-D5-F5)*24</f>
         <v>0</v>
       </c>
@@ -2866,17 +2487,17 @@
         <f aca="false">A5+1</f>
         <v>43074</v>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="22" t="n">
         <f aca="false">A6</f>
         <v>43074</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>50</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="8" t="n">
         <f aca="false">(E6-D6-F6)*24</f>
         <v>0</v>
@@ -2887,17 +2508,17 @@
         <f aca="false">A6+1</f>
         <v>43075</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="22" t="n">
         <f aca="false">A7</f>
         <v>43075</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>50</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="8" t="n">
         <f aca="false">(E7-D7-F7)*24</f>
         <v>0</v>
@@ -2908,17 +2529,17 @@
         <f aca="false">A7+1</f>
         <v>43076</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <f aca="false">A8</f>
         <v>43076</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>50</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="8" t="n">
         <f aca="false">(E8-D8-F8)*24</f>
         <v>0</v>
@@ -2929,17 +2550,17 @@
         <f aca="false">A8+1</f>
         <v>43077</v>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="22" t="n">
         <f aca="false">A9</f>
         <v>43077</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>50</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="8" t="n">
         <f aca="false">(E9-D9-F9)*24</f>
         <v>0</v>
@@ -2950,17 +2571,17 @@
         <f aca="false">A9+1</f>
         <v>43078</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="22" t="n">
         <f aca="false">A10</f>
         <v>43078</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>50</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="8" t="n">
         <f aca="false">(E10-D10-F10)*24</f>
         <v>0</v>
@@ -2972,18 +2593,18 @@
         <f aca="false">A10+1</f>
         <v>43079</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="22" t="n">
         <f aca="false">A11</f>
         <v>43079</v>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="0" t="n">
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>50</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="8" t="n">
         <f aca="false">(E11-D11-F11)*24</f>
         <v>0</v>
       </c>
@@ -2994,18 +2615,18 @@
         <f aca="false">A11+1</f>
         <v>43080</v>
       </c>
-      <c r="B12" s="26" t="n">
+      <c r="B12" s="22" t="n">
         <f aca="false">A12</f>
         <v>43080</v>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="0" t="n">
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>51</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="8" t="n">
         <f aca="false">(E12-D12-F12)*24</f>
         <v>0</v>
       </c>
@@ -3015,17 +2636,17 @@
         <f aca="false">A12+1</f>
         <v>43081</v>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="22" t="n">
         <f aca="false">A13</f>
         <v>43081</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="0" t="n">
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>51</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="8" t="n">
         <f aca="false">(E13-D13-F13)*24</f>
         <v>0</v>
@@ -3036,17 +2657,17 @@
         <f aca="false">A13+1</f>
         <v>43082</v>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="22" t="n">
         <f aca="false">A14</f>
         <v>43082</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>51</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="8" t="n">
         <f aca="false">(E14-D14-F14)*24</f>
         <v>0</v>
@@ -3057,58 +2678,58 @@
         <f aca="false">A14+1</f>
         <v>43083</v>
       </c>
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="22" t="n">
         <f aca="false">A15</f>
         <v>43083</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="0" t="n">
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>51</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="8" t="n">
         <f aca="false">(E15-D15-F15)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="n">
+      <c r="A16" s="24" t="n">
         <f aca="false">A15+1</f>
         <v>43084</v>
       </c>
-      <c r="B16" s="31" t="n">
+      <c r="B16" s="25" t="n">
         <f aca="false">A16</f>
         <v>43084</v>
       </c>
-      <c r="C16" s="32" t="n">
+      <c r="C16" s="1" t="n">
         <f aca="false">WEEKNUM(A16,2)</f>
         <v>51</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+      <c r="D16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <f aca="false">A16+1</f>
         <v>43085</v>
       </c>
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="22" t="n">
         <f aca="false">A17</f>
         <v>43085</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="0" t="n">
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>51</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="8" t="n">
         <f aca="false">(E17-D17-F17)*24</f>
         <v>0</v>
@@ -3120,18 +2741,18 @@
         <f aca="false">A17+1</f>
         <v>43086</v>
       </c>
-      <c r="B18" s="26" t="n">
+      <c r="B18" s="22" t="n">
         <f aca="false">A18</f>
         <v>43086</v>
       </c>
-      <c r="C18" s="27" t="n">
+      <c r="C18" s="0" t="n">
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>51</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29" t="n">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="8" t="n">
         <f aca="false">(E18-D18-F18)*24</f>
         <v>0</v>
       </c>
@@ -3142,18 +2763,18 @@
         <f aca="false">A18+1</f>
         <v>43087</v>
       </c>
-      <c r="B19" s="26" t="n">
+      <c r="B19" s="22" t="n">
         <f aca="false">A19</f>
         <v>43087</v>
       </c>
-      <c r="C19" s="27" t="n">
+      <c r="C19" s="0" t="n">
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>52</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29" t="n">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="8" t="n">
         <f aca="false">(E19-D19-F19)*24</f>
         <v>0</v>
       </c>
@@ -3163,17 +2784,17 @@
         <f aca="false">A19+1</f>
         <v>43088</v>
       </c>
-      <c r="B20" s="24" t="n">
+      <c r="B20" s="22" t="n">
         <f aca="false">A20</f>
         <v>43088</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="0" t="n">
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>52</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="8" t="n">
         <f aca="false">(E20-D20-F20)*24</f>
         <v>0</v>
@@ -3184,17 +2805,17 @@
         <f aca="false">A20+1</f>
         <v>43089</v>
       </c>
-      <c r="B21" s="24" t="n">
+      <c r="B21" s="22" t="n">
         <f aca="false">A21</f>
         <v>43089</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="0" t="n">
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>52</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="8" t="n">
         <f aca="false">(E21-D21-F21)*24</f>
         <v>0</v>
@@ -3205,17 +2826,17 @@
         <f aca="false">A21+1</f>
         <v>43090</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="22" t="n">
         <f aca="false">A22</f>
         <v>43090</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="0" t="n">
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>52</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="8" t="n">
         <f aca="false">(E22-D22-F22)*24</f>
         <v>0</v>
@@ -3226,17 +2847,17 @@
         <f aca="false">A22+1</f>
         <v>43091</v>
       </c>
-      <c r="B23" s="24" t="n">
+      <c r="B23" s="22" t="n">
         <f aca="false">A23</f>
         <v>43091</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="0" t="n">
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>52</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="8" t="n">
         <f aca="false">(E23-D23-F23)*24</f>
         <v>0</v>
@@ -3247,17 +2868,17 @@
         <f aca="false">A23+1</f>
         <v>43092</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="22" t="n">
         <f aca="false">A24</f>
         <v>43092</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="0" t="n">
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>52</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="8" t="n">
         <f aca="false">(E24-D24-F24)*24</f>
         <v>0</v>
@@ -3269,18 +2890,18 @@
         <f aca="false">A24+1</f>
         <v>43093</v>
       </c>
-      <c r="B25" s="26" t="n">
+      <c r="B25" s="22" t="n">
         <f aca="false">A25</f>
         <v>43093</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="0" t="n">
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>52</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29" t="n">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="8" t="n">
         <f aca="false">(E25-D25-F25)*24</f>
         <v>0</v>
       </c>
@@ -3291,18 +2912,18 @@
         <f aca="false">A25+1</f>
         <v>43094</v>
       </c>
-      <c r="B26" s="26" t="n">
+      <c r="B26" s="22" t="n">
         <f aca="false">A26</f>
         <v>43094</v>
       </c>
-      <c r="C26" s="27" t="n">
+      <c r="C26" s="0" t="n">
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>53</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29" t="n">
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="8" t="n">
         <f aca="false">(E26-D26-F26)*24</f>
         <v>0</v>
       </c>
@@ -3312,17 +2933,17 @@
         <f aca="false">A26+1</f>
         <v>43095</v>
       </c>
-      <c r="B27" s="24" t="n">
+      <c r="B27" s="22" t="n">
         <f aca="false">A27</f>
         <v>43095</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="0" t="n">
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>53</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="8" t="n">
         <f aca="false">(E27-D27-F27)*24</f>
         <v>0</v>
@@ -3333,17 +2954,17 @@
         <f aca="false">A27+1</f>
         <v>43096</v>
       </c>
-      <c r="B28" s="24" t="n">
+      <c r="B28" s="22" t="n">
         <f aca="false">A28</f>
         <v>43096</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>53</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="8" t="n">
         <f aca="false">(E28-D28-F28)*24</f>
         <v>0</v>
@@ -3354,17 +2975,17 @@
         <f aca="false">A28+1</f>
         <v>43097</v>
       </c>
-      <c r="B29" s="24" t="n">
+      <c r="B29" s="22" t="n">
         <f aca="false">A29</f>
         <v>43097</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="0" t="n">
         <f aca="false">WEEKNUM(A29,2)</f>
         <v>53</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="8" t="n">
         <f aca="false">(E29-D29-F29)*24</f>
         <v>0</v>
@@ -3375,17 +2996,17 @@
         <f aca="false">A29+1</f>
         <v>43098</v>
       </c>
-      <c r="B30" s="24" t="n">
+      <c r="B30" s="22" t="n">
         <f aca="false">A30</f>
         <v>43098</v>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="0" t="n">
         <f aca="false">WEEKNUM(A30,2)</f>
         <v>53</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="8" t="n">
         <f aca="false">(E30-D30-F30)*24</f>
         <v>0</v>
@@ -3396,17 +3017,17 @@
         <f aca="false">A30+1</f>
         <v>43099</v>
       </c>
-      <c r="B31" s="24" t="n">
+      <c r="B31" s="22" t="n">
         <f aca="false">A31</f>
         <v>43099</v>
       </c>
-      <c r="C31" s="9" t="n">
+      <c r="C31" s="0" t="n">
         <f aca="false">WEEKNUM(A31,2)</f>
         <v>53</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="8" t="n">
         <f aca="false">(E31-D31-F31)*24</f>
         <v>0</v>
@@ -3414,32 +3035,32 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35" t="n">
+      <c r="A32" s="28" t="n">
         <f aca="false">A31+1</f>
         <v>43100</v>
       </c>
-      <c r="B32" s="36" t="n">
+      <c r="B32" s="29" t="n">
         <f aca="false">A32</f>
         <v>43100</v>
       </c>
-      <c r="C32" s="37" t="n">
+      <c r="C32" s="30" t="n">
         <f aca="false">WEEKNUM(A32,2)</f>
         <v>53</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39" t="n">
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32" t="n">
         <f aca="false">(E32-D32-F32)*24</f>
         <v>0</v>
       </c>
-      <c r="H32" s="39"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="40"/>
+      <c r="A33" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="33"/>
       <c r="C33" s="0" t="n">
         <f aca="false">4*Zusammenfassung!B1</f>
         <v>36</v>
@@ -3447,19 +3068,19 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43" t="n">
+      <c r="A34" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="43"/>
+      <c r="H34" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3470,58 +3091,53 @@
   <conditionalFormatting sqref="B2:C32">
     <cfRule type="timePeriod" priority="2" timePeriod="yesterday" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G15,A17:G32,A16:D16">
+  <conditionalFormatting sqref="H25">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>WEEKDAY($A2,2) &gt; 5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A25,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A31,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>WEEKDAY($A24,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>WEEKDAY($A18,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>WEEKDAY($A11,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>WEEKDAY($A10,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>WEEKDAY($A4,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>WEEKDAY($A3,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3548,59 +3164,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.88148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="49"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <f aca="false">DATE(2018,1,1)</f>
         <v>43101</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="22" t="n">
         <f aca="false">A2</f>
         <v>43101</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="0" t="n">
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="8" t="n">
         <v>0</v>
       </c>
@@ -3610,17 +3226,17 @@
         <f aca="false">A2+1</f>
         <v>43102</v>
       </c>
-      <c r="B3" s="24" t="n">
+      <c r="B3" s="22" t="n">
         <f aca="false">A3</f>
         <v>43102</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="0" t="n">
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="8" t="n">
         <f aca="false">(E3-D3-F3)*24</f>
         <v>0</v>
@@ -3631,18 +3247,18 @@
         <f aca="false">A3+1</f>
         <v>43103</v>
       </c>
-      <c r="B4" s="26" t="n">
+      <c r="B4" s="22" t="n">
         <f aca="false">A4</f>
         <v>43103</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="0" t="n">
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29" t="n">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="8" t="n">
         <f aca="false">(E4-D4-F4)*24</f>
         <v>0</v>
       </c>
@@ -3652,18 +3268,18 @@
         <f aca="false">A4+1</f>
         <v>43104</v>
       </c>
-      <c r="B5" s="26" t="n">
+      <c r="B5" s="22" t="n">
         <f aca="false">A5</f>
         <v>43104</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="0" t="n">
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29" t="n">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="8" t="n">
         <f aca="false">(E5-D5-F5)*24</f>
         <v>0</v>
       </c>
@@ -3673,18 +3289,18 @@
         <f aca="false">A5+1</f>
         <v>43105</v>
       </c>
-      <c r="B6" s="24" t="n">
+      <c r="B6" s="22" t="n">
         <f aca="false">A6</f>
         <v>43105</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="0" t="n">
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="29" t="n">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="8" t="n">
         <f aca="false">(E6-D6-F6)*24</f>
         <v>0</v>
       </c>
@@ -3694,18 +3310,18 @@
         <f aca="false">A6+1</f>
         <v>43106</v>
       </c>
-      <c r="B7" s="24" t="n">
+      <c r="B7" s="22" t="n">
         <f aca="false">A7</f>
         <v>43106</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="0" t="n">
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="29" t="n">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="8" t="n">
         <f aca="false">(E7-D7-F7)*24</f>
         <v>0</v>
       </c>
@@ -3716,17 +3332,17 @@
         <f aca="false">A7+1</f>
         <v>43107</v>
       </c>
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="22" t="n">
         <f aca="false">A8</f>
         <v>43107</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="0" t="n">
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="8" t="n">
         <f aca="false">(E8-D8-F8)*24</f>
         <v>0</v>
@@ -3738,17 +3354,17 @@
         <f aca="false">A8+1</f>
         <v>43108</v>
       </c>
-      <c r="B9" s="24" t="n">
+      <c r="B9" s="22" t="n">
         <f aca="false">A9</f>
         <v>43108</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="0" t="n">
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="8" t="n">
         <f aca="false">(E9-D9-F9)*24</f>
         <v>0</v>
@@ -3759,17 +3375,17 @@
         <f aca="false">A9+1</f>
         <v>43109</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="22" t="n">
         <f aca="false">A10</f>
         <v>43109</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="0" t="n">
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="8" t="n">
         <f aca="false">(E10-D10-F10)*24</f>
         <v>0</v>
@@ -3780,18 +3396,18 @@
         <f aca="false">A10+1</f>
         <v>43110</v>
       </c>
-      <c r="B11" s="26" t="n">
+      <c r="B11" s="22" t="n">
         <f aca="false">A11</f>
         <v>43110</v>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="0" t="n">
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>2</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29" t="n">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="8" t="n">
         <f aca="false">(E11-D11-F11)*24</f>
         <v>0</v>
       </c>
@@ -3801,58 +3417,58 @@
         <f aca="false">A11+1</f>
         <v>43111</v>
       </c>
-      <c r="B12" s="26" t="n">
+      <c r="B12" s="22" t="n">
         <f aca="false">A12</f>
         <v>43111</v>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="0" t="n">
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>2</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29" t="n">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="8" t="n">
         <f aca="false">(E12-D12-F12)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="n">
+      <c r="A13" s="24" t="n">
         <f aca="false">A12+1</f>
         <v>43112</v>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="25" t="n">
         <f aca="false">A13</f>
         <v>43112</v>
       </c>
-      <c r="C13" s="32" t="n">
+      <c r="C13" s="1" t="n">
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>2</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="D13" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <f aca="false">A13+1</f>
         <v>43113</v>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="22" t="n">
         <f aca="false">A14</f>
         <v>43113</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>2</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="8" t="n">
         <f aca="false">(E14-D14-F14)*24</f>
         <v>0</v>
@@ -3864,17 +3480,17 @@
         <f aca="false">A14+1</f>
         <v>43114</v>
       </c>
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="22" t="n">
         <f aca="false">A15</f>
         <v>43114</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="0" t="n">
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>2</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="8" t="n">
         <f aca="false">(E15-D15-F15)*24</f>
         <v>0</v>
@@ -3886,17 +3502,17 @@
         <f aca="false">A15+1</f>
         <v>43115</v>
       </c>
-      <c r="B16" s="24" t="n">
+      <c r="B16" s="22" t="n">
         <f aca="false">A16</f>
         <v>43115</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="0" t="n">
         <f aca="false">WEEKNUM(A16,2)</f>
         <v>3</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="8" t="n">
         <f aca="false">(E16-D16-F16)*24</f>
         <v>0</v>
@@ -3907,17 +3523,17 @@
         <f aca="false">A16+1</f>
         <v>43116</v>
       </c>
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="22" t="n">
         <f aca="false">A17</f>
         <v>43116</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="0" t="n">
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>3</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="8" t="n">
         <f aca="false">(E17-D17-F17)*24</f>
         <v>0</v>
@@ -3928,18 +3544,18 @@
         <f aca="false">A17+1</f>
         <v>43117</v>
       </c>
-      <c r="B18" s="26" t="n">
+      <c r="B18" s="22" t="n">
         <f aca="false">A18</f>
         <v>43117</v>
       </c>
-      <c r="C18" s="27" t="n">
+      <c r="C18" s="0" t="n">
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>3</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29" t="n">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="8" t="n">
         <f aca="false">(E18-D18-F18)*24</f>
         <v>0</v>
       </c>
@@ -3949,58 +3565,58 @@
         <f aca="false">A18+1</f>
         <v>43118</v>
       </c>
-      <c r="B19" s="26" t="n">
+      <c r="B19" s="22" t="n">
         <f aca="false">A19</f>
         <v>43118</v>
       </c>
-      <c r="C19" s="27" t="n">
+      <c r="C19" s="0" t="n">
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>3</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29" t="n">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="8" t="n">
         <f aca="false">(E19-D19-F19)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="n">
+      <c r="A20" s="24" t="n">
         <f aca="false">A19+1</f>
         <v>43119</v>
       </c>
-      <c r="B20" s="31" t="n">
+      <c r="B20" s="25" t="n">
         <f aca="false">A20</f>
         <v>43119</v>
       </c>
-      <c r="C20" s="32" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>3</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
+      <c r="D20" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <f aca="false">A20+1</f>
         <v>43120</v>
       </c>
-      <c r="B21" s="24" t="n">
+      <c r="B21" s="22" t="n">
         <f aca="false">A21</f>
         <v>43120</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="0" t="n">
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>3</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="8" t="n">
         <f aca="false">(E21-D21-F21)*24</f>
         <v>0</v>
@@ -4012,17 +3628,17 @@
         <f aca="false">A21+1</f>
         <v>43121</v>
       </c>
-      <c r="B22" s="24" t="n">
+      <c r="B22" s="22" t="n">
         <f aca="false">A22</f>
         <v>43121</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="0" t="n">
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>3</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="8" t="n">
         <f aca="false">(E22-D22-F22)*24</f>
         <v>0</v>
@@ -4034,17 +3650,17 @@
         <f aca="false">A22+1</f>
         <v>43122</v>
       </c>
-      <c r="B23" s="24" t="n">
+      <c r="B23" s="22" t="n">
         <f aca="false">A23</f>
         <v>43122</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="0" t="n">
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>4</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="8" t="n">
         <f aca="false">(E23-D23-F23)*24</f>
         <v>0</v>
@@ -4055,17 +3671,17 @@
         <f aca="false">A23+1</f>
         <v>43123</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="22" t="n">
         <f aca="false">A24</f>
         <v>43123</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="0" t="n">
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>4</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="8" t="n">
         <f aca="false">(E24-D24-F24)*24</f>
         <v>0</v>
@@ -4076,18 +3692,18 @@
         <f aca="false">A24+1</f>
         <v>43124</v>
       </c>
-      <c r="B25" s="26" t="n">
+      <c r="B25" s="22" t="n">
         <f aca="false">A25</f>
         <v>43124</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="0" t="n">
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>4</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29" t="n">
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="8" t="n">
         <f aca="false">(E25-D25-F25)*24</f>
         <v>0</v>
       </c>
@@ -4097,18 +3713,18 @@
         <f aca="false">A25+1</f>
         <v>43125</v>
       </c>
-      <c r="B26" s="26" t="n">
+      <c r="B26" s="22" t="n">
         <f aca="false">A26</f>
         <v>43125</v>
       </c>
-      <c r="C26" s="27" t="n">
+      <c r="C26" s="0" t="n">
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>4</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29" t="n">
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="8" t="n">
         <f aca="false">(E26-D26-F26)*24</f>
         <v>0</v>
       </c>
@@ -4118,17 +3734,17 @@
         <f aca="false">A26+1</f>
         <v>43126</v>
       </c>
-      <c r="B27" s="24" t="n">
+      <c r="B27" s="22" t="n">
         <f aca="false">A27</f>
         <v>43126</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="0" t="n">
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>4</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="8" t="n">
         <f aca="false">(E27-D27-F27)*24</f>
         <v>0</v>
@@ -4139,17 +3755,17 @@
         <f aca="false">A27+1</f>
         <v>43127</v>
       </c>
-      <c r="B28" s="24" t="n">
+      <c r="B28" s="22" t="n">
         <f aca="false">A28</f>
         <v>43127</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>4</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="8" t="n">
         <f aca="false">(E28-D28-F28)*24</f>
         <v>0</v>
@@ -4161,17 +3777,17 @@
         <f aca="false">A28+1</f>
         <v>43128</v>
       </c>
-      <c r="B29" s="24" t="n">
+      <c r="B29" s="22" t="n">
         <f aca="false">A29</f>
         <v>43128</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="0" t="n">
         <f aca="false">WEEKNUM(A29,2)</f>
         <v>4</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="8" t="n">
         <f aca="false">(E29-D29-F29)*24</f>
         <v>0</v>
@@ -4183,17 +3799,17 @@
         <f aca="false">A29+1</f>
         <v>43129</v>
       </c>
-      <c r="B30" s="24" t="n">
+      <c r="B30" s="22" t="n">
         <f aca="false">A30</f>
         <v>43129</v>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="0" t="n">
         <f aca="false">WEEKNUM(A30,2)</f>
         <v>5</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="8" t="n">
         <f aca="false">(E30-D30-F30)*24</f>
         <v>0</v>
@@ -4204,49 +3820,49 @@
         <f aca="false">A30+1</f>
         <v>43130</v>
       </c>
-      <c r="B31" s="24" t="n">
+      <c r="B31" s="22" t="n">
         <f aca="false">A31</f>
         <v>43130</v>
       </c>
-      <c r="C31" s="9" t="n">
+      <c r="C31" s="0" t="n">
         <f aca="false">WEEKNUM(A31,2)</f>
         <v>5</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="8" t="n">
         <f aca="false">(E31-D31-F31)*24</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35" t="n">
+      <c r="A32" s="28" t="n">
         <f aca="false">A31+1</f>
         <v>43131</v>
       </c>
-      <c r="B32" s="36" t="n">
+      <c r="B32" s="29" t="n">
         <f aca="false">A32</f>
         <v>43131</v>
       </c>
-      <c r="C32" s="37" t="n">
+      <c r="C32" s="30" t="n">
         <f aca="false">WEEKNUM(A32,2)</f>
         <v>5</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39" t="n">
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32" t="n">
         <f aca="false">(E32-D32-F32)*24</f>
         <v>0</v>
       </c>
-      <c r="H32" s="39"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="40"/>
+      <c r="A33" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="33"/>
       <c r="C33" s="0" t="n">
         <f aca="false">5*Zusammenfassung!B1</f>
         <v>45</v>
@@ -4254,19 +3870,19 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43" t="n">
+      <c r="A34" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="36" t="n">
         <f aca="false">SUM(G2:G32)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="43"/>
+      <c r="H34" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4278,53 +3894,48 @@
   <conditionalFormatting sqref="B2:C32">
     <cfRule type="timePeriod" priority="2" timePeriod="yesterday" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:G12,A21:G32,A20:D20,A14:G19,A13:D13">
+  <conditionalFormatting sqref="H8">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>WEEKDAY($A2,2) &gt; 5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A8,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>WEEKDAY($A7,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>WEEKDAY($A14,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>WEEKDAY($A15,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>WEEKDAY($A21,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>WEEKDAY($A22,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>WEEKDAY($A29,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>WEEKDAY($A28,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>